<commit_message>
PROS-5380 - Error in sanofieg
-- fixed --
</commit_message>
<xml_diff>
--- a/Projects/SANOFIEG/Data/Template.xlsx
+++ b/Projects/SANOFIEG/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$I$11</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$H$2</definedName>
-    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">MSL!$A$2:$I$11</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">MSL!$A$2:$I$11</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">MSL!$A$2:$I$11</definedName>
@@ -45,6 +45,9 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$I$11</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$I$11</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$I$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">MSL!$A$2:$I$11</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary Shelf_Location'!$A$2:$H$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$H$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$H$2</definedName>
@@ -69,6 +72,9 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$H$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$H$2</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$H$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$H$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$H$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary Shelf_Location'!$A$2:$H$2</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Primary_Brand_Blocking!$B$4:$I$8</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
@@ -79,31 +85,34 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$H$11</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Primary&amp;Secondary_Facings'!$A$2:$G$11</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -115,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="65">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -138,28 +147,10 @@
     <t xml:space="preserve">SCORE</t>
   </si>
   <si>
-    <t xml:space="preserve">POSM Availability Primary</t>
+    <t xml:space="preserve">Blocked Together</t>
   </si>
   <si>
     <t xml:space="preserve">Primary Shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Availability Per SKU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primary&amp;Secondary_POSM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">numeric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POSM Availability Secondary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary Shelf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blocked Together</t>
   </si>
   <si>
     <t xml:space="preserve">Blocked Together Per Brand</t>
@@ -168,10 +159,16 @@
     <t xml:space="preserve">Primary_Brand_Blocking</t>
   </si>
   <si>
+    <t xml:space="preserve">numeric</t>
+  </si>
+  <si>
     <t xml:space="preserve">MSL Compliance</t>
   </si>
   <si>
     <t xml:space="preserve">MSL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Availability Per SKU</t>
   </si>
   <si>
     <t xml:space="preserve">Perfect Store</t>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t xml:space="preserve">Product Minimum Facings Secondary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary Shelf</t>
   </si>
   <si>
     <t xml:space="preserve">Primary Shelf Compliance</t>
@@ -1321,21 +1321,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.4858299595142"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.54655870445344"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.6882591093117"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2591093117409"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="44.4412955465587"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="44.3198380566802"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.54655870445344"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.2995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.91093117408907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0364372469636"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.3441295546559"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="47.7449392712551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="47.6234817813765"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.91093117408907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,184 +1382,144 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+    <row r="3" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+    <row r="4" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="D4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="E7" s="13"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="27.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1585,15 +1545,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="52.7651821862348"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="113.975708502024"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4412955465587"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.5263157894737"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="56.6801619433198"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="122.542510121458"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.7692307692308"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6234817813765"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.914979757085"/>
     <col collapsed="false" hidden="true" max="6" min="6" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="20.6882591093117"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.5263157894737"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="22.0364372469636"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.6234817813765"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.4048582995951"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="41.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1605,7 +1565,7 @@
       <c r="F1" s="26"/>
       <c r="G1" s="26"/>
       <c r="H1" s="27" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
@@ -1615,48 +1575,48 @@
         <v>0</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="F2" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="G2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="H2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="I2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="J2" s="32" t="s">
         <v>33</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" s="35" t="n">
         <v>3582910014812</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E3" s="36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F3" s="37"/>
       <c r="G3" s="38" t="n">
@@ -1674,19 +1634,19 @@
     </row>
     <row r="4" customFormat="false" ht="24.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" s="35" t="n">
         <v>3582910014829</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F4" s="40"/>
       <c r="G4" s="41" t="n">
@@ -1704,19 +1664,19 @@
     </row>
     <row r="5" s="42" customFormat="true" ht="64.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" s="35" t="n">
         <v>3582910073840</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F5" s="40"/>
       <c r="G5" s="41" t="n">
@@ -1734,19 +1694,19 @@
     </row>
     <row r="6" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="35" t="n">
         <v>6223003990374</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F6" s="43"/>
       <c r="G6" s="41" t="n">
@@ -1764,19 +1724,19 @@
     </row>
     <row r="7" customFormat="false" ht="33.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="35" t="n">
         <v>6223003992002</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="45" t="n">
@@ -1794,19 +1754,19 @@
     </row>
     <row r="8" customFormat="false" ht="33.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" s="35" t="n">
         <v>6223003991364</v>
       </c>
       <c r="D8" s="34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F8" s="43"/>
       <c r="G8" s="41" t="n">
@@ -1824,19 +1784,19 @@
     </row>
     <row r="9" customFormat="false" ht="33.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="35" t="n">
         <v>6223003991388</v>
       </c>
       <c r="D9" s="34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F9" s="37"/>
       <c r="G9" s="41" t="n">
@@ -1854,19 +1814,19 @@
     </row>
     <row r="10" customFormat="false" ht="33.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="35" t="n">
         <v>6223003991715</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F10" s="37"/>
       <c r="G10" s="45" t="n">
@@ -1884,19 +1844,19 @@
     </row>
     <row r="11" customFormat="false" ht="33.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="33" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" s="35" t="n">
         <v>6223003991906</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F11" s="43"/>
       <c r="G11" s="45" t="n">
@@ -1942,15 +1902,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="46" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="15.919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="46" width="16.4048582995951"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="46" width="39.5425101214575"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="29.2591093117409"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="46" width="12.4817813765182"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="46" width="10.0404858299595"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="46" width="13.3481781376518"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="46" width="10.4048582995951"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="46" width="29.2591093117409"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="16.8947368421053"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="46" width="17.502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="46" width="42.3562753036437"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="31.3441295546559"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="46" width="13.2267206477733"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="46" width="10.4048582995951"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="46" width="14.4453441295547"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="46" width="10.7773279352227"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1961,7 +1921,7 @@
       <c r="E1" s="26"/>
       <c r="F1" s="26"/>
       <c r="G1" s="47" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H1" s="47"/>
       <c r="I1" s="0"/>
@@ -1971,31 +1931,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E2" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="49" t="s">
-        <v>32</v>
-      </c>
       <c r="G2" s="50" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H2" s="51" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I2" s="52"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B3" s="54"/>
       <c r="C3" s="54"/>
@@ -2007,7 +1967,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B4" s="54"/>
       <c r="C4" s="54"/>
@@ -2019,7 +1979,7 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" s="54"/>
       <c r="C5" s="54"/>
@@ -2031,7 +1991,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B6" s="54"/>
       <c r="C6" s="54"/>
@@ -2043,7 +2003,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
@@ -2055,7 +2015,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B8" s="54"/>
       <c r="C8" s="54"/>
@@ -2067,7 +2027,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B9" s="54"/>
       <c r="C9" s="54"/>
@@ -2079,7 +2039,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B10" s="54"/>
       <c r="C10" s="54"/>
@@ -2091,7 +2051,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B11" s="54"/>
       <c r="C11" s="54"/>
@@ -2103,7 +2063,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B12" s="54"/>
       <c r="C12" s="54"/>
@@ -2115,7 +2075,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B13" s="54"/>
       <c r="C13" s="54"/>
@@ -2127,7 +2087,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B14" s="54"/>
       <c r="C14" s="54"/>
@@ -2139,7 +2099,7 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B15" s="54"/>
       <c r="C15" s="54"/>
@@ -2151,7 +2111,7 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B16" s="54"/>
       <c r="C16" s="54"/>
@@ -2163,7 +2123,7 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="53" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B17" s="54"/>
       <c r="C17" s="54"/>
@@ -2175,7 +2135,7 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="61" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B18" s="62"/>
       <c r="C18" s="62"/>
@@ -2209,20 +2169,20 @@
   </sheetPr>
   <dimension ref="1:18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="46" width="16.8947368421053"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="15.668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="46" width="14.2024291497976"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="46" width="35.748987854251"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="25.9514170040486"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="46" width="20.3238866396761"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="46" width="23.0161943319838"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="46" width="10.4048582995951"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="46" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="16.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="46" width="15.1821862348178"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="46" width="38.4412955465587"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="27.9068825910931"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="46" width="21.5465587044534"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="46" width="24.6072874493927"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="46" width="10.7773279352227"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,7 +2193,7 @@
       <c r="E1" s="26"/>
       <c r="F1" s="26"/>
       <c r="G1" s="67" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H1" s="67"/>
       <c r="I1" s="67"/>
@@ -3258,28 +3218,28 @@
         <v>0</v>
       </c>
       <c r="B2" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="G2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="49" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="30" t="s">
+      <c r="H2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="32" t="s">
         <v>33</v>
-      </c>
-      <c r="G2" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>36</v>
       </c>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
@@ -4299,19 +4259,19 @@
     </row>
     <row r="3" customFormat="false" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="68" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B3" s="69" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D3" s="69" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E3" s="70" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F3" s="71" t="n">
         <v>1</v>
@@ -5343,19 +5303,19 @@
     </row>
     <row r="4" customFormat="false" ht="28.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="68" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" s="69" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E4" s="70" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F4" s="71" t="n">
         <v>1</v>
@@ -6387,16 +6347,16 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="68" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5" s="73" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C5" s="73" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D5" s="73" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E5" s="74" t="n">
         <v>6223003990374</v>
@@ -6416,16 +6376,16 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="68" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D6" s="73" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E6" s="74" t="n">
         <v>6223003992002</v>
@@ -6445,19 +6405,19 @@
     </row>
     <row r="7" customFormat="false" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="68" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B7" s="69" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C7" s="69" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D7" s="69" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E7" s="70" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F7" s="71" t="n">
         <v>1</v>
@@ -6474,16 +6434,16 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="68" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B8" s="73" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C8" s="73" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D8" s="73" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E8" s="74" t="n">
         <v>6223003991906</v>
@@ -6554,17 +6514,17 @@
   <dimension ref="A1:G65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="52.7651821862348"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.8097165991903"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4412955465587"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5263157894737"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="56.6801619433198"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.6518218623482"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.7692307692308"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6234817813765"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.4048582995951"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6574,7 +6534,7 @@
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
       <c r="F1" s="79" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G1" s="79"/>
     </row>
@@ -6583,28 +6543,26 @@
         <v>0</v>
       </c>
       <c r="B2" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="81" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="81" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="81" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="81" t="s">
-        <v>31</v>
-      </c>
       <c r="F2" s="82" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G2" s="83" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="84" t="s">
-        <v>7</v>
-      </c>
+      <c r="A3" s="84"/>
       <c r="B3" s="85"/>
       <c r="C3" s="86"/>
       <c r="D3" s="86"/>
@@ -6613,9 +6571,7 @@
       <c r="G3" s="88"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="89" t="s">
-        <v>12</v>
-      </c>
+      <c r="A4" s="89"/>
       <c r="B4" s="85"/>
       <c r="C4" s="86"/>
       <c r="D4" s="86"/>
@@ -6624,9 +6580,7 @@
       <c r="G4" s="90"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="89" t="s">
-        <v>12</v>
-      </c>
+      <c r="A5" s="89"/>
       <c r="B5" s="85"/>
       <c r="C5" s="86"/>
       <c r="D5" s="86"/>
@@ -6635,9 +6589,7 @@
       <c r="G5" s="90"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="89" t="s">
-        <v>12</v>
-      </c>
+      <c r="A6" s="89"/>
       <c r="B6" s="85"/>
       <c r="C6" s="86"/>
       <c r="D6" s="86"/>
@@ -6646,9 +6598,7 @@
       <c r="G6" s="90"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="89" t="s">
-        <v>12</v>
-      </c>
+      <c r="A7" s="89"/>
       <c r="B7" s="85"/>
       <c r="C7" s="86"/>
       <c r="D7" s="86"/>
@@ -6657,9 +6607,7 @@
       <c r="G7" s="90"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="89" t="s">
-        <v>12</v>
-      </c>
+      <c r="A8" s="89"/>
       <c r="B8" s="85"/>
       <c r="C8" s="86"/>
       <c r="D8" s="86"/>
@@ -6668,9 +6616,7 @@
       <c r="G8" s="90"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="89" t="s">
-        <v>12</v>
-      </c>
+      <c r="A9" s="89"/>
       <c r="B9" s="85"/>
       <c r="C9" s="86"/>
       <c r="D9" s="85"/>
@@ -6679,9 +6625,7 @@
       <c r="G9" s="92"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="93" t="s">
-        <v>12</v>
-      </c>
+      <c r="A10" s="93"/>
       <c r="B10" s="94"/>
       <c r="C10" s="95"/>
       <c r="D10" s="94"/>
@@ -6728,15 +6672,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.4777327935223"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.3724696356275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="62.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.4412955465587"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5263157894737"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="20.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.5263157894737"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="58.8866396761134"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.0404858299595"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8056680161943"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="63.8987854251012"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="67.085020242915"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.7692307692308"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.6234817813765"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6234817813765"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="63.412955465587"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.4048582995951"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6747,7 +6691,7 @@
       <c r="E1" s="25"/>
       <c r="F1" s="26"/>
       <c r="G1" s="96" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="H1" s="96"/>
       <c r="I1" s="96"/>
@@ -6757,45 +6701,45 @@
         <v>0</v>
       </c>
       <c r="B2" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="F2" s="98" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="29" t="s">
+      <c r="G2" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="98" t="s">
+      <c r="H2" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>35</v>
-      </c>
       <c r="I2" s="32" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="60" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="84" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B3" s="99" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C3" s="100" t="n">
         <v>3582910014812</v>
       </c>
       <c r="D3" s="99" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E3" s="99" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F3" s="101" t="n">
         <v>1</v>
@@ -6812,19 +6756,19 @@
     </row>
     <row r="4" customFormat="false" ht="48.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="84" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" s="100" t="n">
         <v>3582910014829</v>
       </c>
       <c r="D4" s="99" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E4" s="99" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F4" s="101" t="n">
         <v>1</v>
@@ -6841,19 +6785,19 @@
     </row>
     <row r="5" s="42" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="84" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5" s="99" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C5" s="100" t="n">
         <v>3582910073840</v>
       </c>
       <c r="D5" s="99" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E5" s="99" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F5" s="101" t="n">
         <v>1</v>
@@ -6870,19 +6814,19 @@
     </row>
     <row r="6" s="42" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="84" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="99" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="100" t="n">
         <v>6223003990374</v>
       </c>
       <c r="D6" s="99" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="99" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F6" s="101" t="n">
         <v>1</v>
@@ -6899,19 +6843,19 @@
     </row>
     <row r="7" s="42" customFormat="true" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="84" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" s="99" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="100" t="n">
         <v>6223003992002</v>
       </c>
       <c r="D7" s="99" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E7" s="99" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F7" s="101" t="n">
         <v>1</v>
@@ -6928,19 +6872,19 @@
     </row>
     <row r="8" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="84" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" s="100" t="n">
         <v>6223003991364</v>
       </c>
       <c r="D8" s="99" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E8" s="99" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F8" s="101" t="n">
         <v>1</v>
@@ -6957,19 +6901,19 @@
     </row>
     <row r="9" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="84" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B9" s="99" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" s="100" t="n">
         <v>6223003991388</v>
       </c>
       <c r="D9" s="99" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E9" s="99" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F9" s="101" t="n">
         <v>1</v>
@@ -6986,19 +6930,19 @@
     </row>
     <row r="10" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="84" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B10" s="99" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="100" t="n">
         <v>6223003991715</v>
       </c>
       <c r="D10" s="99" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E10" s="99" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F10" s="101" t="n">
         <v>1</v>
@@ -7015,22 +6959,22 @@
     </row>
     <row r="11" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="105" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11" s="106" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" s="107" t="n">
         <v>6223003991906</v>
       </c>
       <c r="D11" s="106" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E11" s="106" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F11" s="108" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G11" s="109" t="n">
         <v>2</v>
@@ -7130,7 +7074,7 @@
     <row r="1048575" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A2:H11"/>
+  <autoFilter ref="A2:G11"/>
   <mergeCells count="1">
     <mergeCell ref="G1:I1"/>
   </mergeCells>

</xml_diff>